<commit_message>
Update datalist column names
</commit_message>
<xml_diff>
--- a/data-raw/Datalist_e.xlsx
+++ b/data-raw/Datalist_e.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6775CE2-F1DB-4F32-B593-3D7EC5D006DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0B431A-EED5-40BA-89AF-A2252A983A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="660" windowWidth="21600" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7845" windowWidth="28800" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_sheet_template" sheetId="1" r:id="rId1"/>
@@ -28,28 +28,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Key</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(personnel number, ID, AHV)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Age</t>
     </r>
     <r>
@@ -289,6 +267,28 @@
   </si>
   <si>
     <t>Additional information5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(personnel number, ID, etc.)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -838,7 +838,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="2" customWidth="1"/>
@@ -862,73 +862,73 @@
   <sheetData>
     <row r="1" spans="1:23" customFormat="1" ht="168.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:23" customFormat="1" x14ac:dyDescent="0.2"/>

</xml_diff>